<commit_message>
Update BROObject - GMW IMBRO toelichting NL (v1.x).xlsx
</commit_message>
<xml_diff>
--- a/GMW/BROObject - GMW IMBRO toelichting NL (v1.x).xlsx
+++ b/GMW/BROObject - GMW IMBRO toelichting NL (v1.x).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://3hydro-my.sharepoint.com/personal/jos_von_asmuth_3hydro_nl/Documents/GitHub/BRO-Spreadsheet-en-tabelformat/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trefo\OneDrive - Trefoil Hydrology\GitHub\BRO-Spreadsheet-en-tabelformat\GMW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{97183503-7DB5-4199-B0DC-3642120556F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{30C3084F-137C-4A77-855F-1350A758B809}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EDF6D0F-3A3A-40D7-A8DC-8A40DB7B894E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C7958186-5914-4A27-A45D-7A94CBD87F04}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="5" xr2:uid="{C7958186-5914-4A27-A45D-7A94CBD87F04}"/>
   </bookViews>
   <sheets>
     <sheet name="Toelichting" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="306">
   <si>
     <t>deliveryContext</t>
   </si>
@@ -675,9 +675,6 @@
   </si>
   <si>
     <t>De lengte van het deel van de monitoringbuis met perforaties.</t>
-  </si>
-  <si>
-    <t>De lengte van het stijgbuisdeel van de monitoringbuis</t>
   </si>
   <si>
     <t>De lengte van het ingeplaatste stijgbuisdeel.</t>
@@ -1068,6 +1065,15 @@
   </si>
   <si>
     <t>Coördinatenpaar</t>
+  </si>
+  <si>
+    <t>De lengte van de zandvang.</t>
+  </si>
+  <si>
+    <t>De lengte van het stijgbuisdeel van de monitoringbuis.</t>
+  </si>
+  <si>
+    <t>buismateriaal</t>
   </si>
 </sst>
 </file>
@@ -2077,10 +2083,10 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="71" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" s="72" t="s">
         <v>251</v>
-      </c>
-      <c r="B1" s="72" t="s">
-        <v>252</v>
       </c>
       <c r="C1" s="72"/>
       <c r="D1" s="72"/>
@@ -2093,7 +2099,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="75" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B2" s="91">
         <v>1.01</v>
@@ -2109,10 +2115,10 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="75" t="s">
+        <v>253</v>
+      </c>
+      <c r="B3" s="78" t="s">
         <v>254</v>
-      </c>
-      <c r="B3" s="78" t="s">
-        <v>255</v>
       </c>
       <c r="C3" s="76"/>
       <c r="D3" s="76"/>
@@ -2125,10 +2131,10 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="75" t="s">
+        <v>255</v>
+      </c>
+      <c r="B4" s="76" t="s">
         <v>256</v>
-      </c>
-      <c r="B4" s="76" t="s">
-        <v>257</v>
       </c>
       <c r="C4" s="76"/>
       <c r="D4" s="76"/>
@@ -2141,22 +2147,22 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="75" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B5" s="76" t="s">
+        <v>270</v>
+      </c>
+      <c r="C5" s="76" t="s">
         <v>271</v>
       </c>
-      <c r="C5" s="76" t="s">
+      <c r="D5" s="76" t="s">
+        <v>274</v>
+      </c>
+      <c r="E5" s="76" t="s">
+        <v>273</v>
+      </c>
+      <c r="F5" s="79" t="s">
         <v>272</v>
-      </c>
-      <c r="D5" s="76" t="s">
-        <v>275</v>
-      </c>
-      <c r="E5" s="76" t="s">
-        <v>274</v>
-      </c>
-      <c r="F5" s="79" t="s">
-        <v>273</v>
       </c>
       <c r="H5" s="77"/>
       <c r="I5" s="74"/>
@@ -2164,10 +2170,10 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="75" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B6" s="80" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C6" s="76"/>
       <c r="D6" s="76"/>
@@ -2180,10 +2186,10 @@
     </row>
     <row r="7" spans="1:10" ht="15" thickBot="1">
       <c r="A7" s="81" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B7" s="82" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C7" s="82"/>
       <c r="D7" s="82"/>
@@ -2196,37 +2202,37 @@
     </row>
     <row r="9" spans="1:10" ht="23.4">
       <c r="A9" s="84" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="85" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="85" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="85" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="85" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="85" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="85" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="10.199999999999999" customHeight="1">
@@ -2234,13 +2240,13 @@
     </row>
     <row r="17" spans="1:1" ht="23.4">
       <c r="A17" s="84" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="7.8" customHeight="1"/>
     <row r="33" spans="1:1" ht="23.4">
       <c r="A33" s="84" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -2260,8 +2266,8 @@
   </sheetPr>
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2307,25 +2313,25 @@
         <v>122</v>
       </c>
       <c r="B2" s="29" t="s">
+        <v>276</v>
+      </c>
+      <c r="C2" s="29" t="s">
         <v>277</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="D2" s="17" t="s">
+        <v>275</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>278</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>276</v>
-      </c>
-      <c r="E2" s="18" t="s">
+      <c r="F2" s="30" t="s">
         <v>279</v>
-      </c>
-      <c r="F2" s="30" t="s">
-        <v>280</v>
       </c>
       <c r="G2" s="31">
         <v>1</v>
       </c>
       <c r="H2" s="89" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2349,7 +2355,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="32" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2371,7 +2377,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2380,7 +2386,7 @@
         <v>150</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>0</v>
@@ -2389,7 +2395,7 @@
         <v>118</v>
       </c>
       <c r="F5" s="30" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G5" s="31">
         <v>1</v>
@@ -2404,7 +2410,7 @@
         <v>151</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>1</v>
@@ -2419,7 +2425,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="32" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="28.8">
@@ -2428,7 +2434,7 @@
         <v>152</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>2</v>
@@ -2452,7 +2458,7 @@
         <v>157</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D8" s="67" t="s">
         <v>112</v>
@@ -2474,7 +2480,7 @@
         <v>158</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D9" s="67" t="s">
         <v>113</v>
@@ -2489,7 +2495,7 @@
         <v>147</v>
       </c>
       <c r="H9" s="32" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -2513,7 +2519,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="32" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="28.8">
@@ -2522,7 +2528,7 @@
         <v>165</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D11" s="67" t="s">
         <v>129</v>
@@ -2583,7 +2589,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="39" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -2594,7 +2600,7 @@
         <v>141</v>
       </c>
       <c r="C14" s="40" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>123</v>
@@ -2618,7 +2624,7 @@
         <v>142</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>4</v>
@@ -2657,7 +2663,7 @@
         <v>1</v>
       </c>
       <c r="H16" s="39" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2668,7 +2674,7 @@
         <v>138</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>131</v>
@@ -2692,7 +2698,7 @@
         <v>139</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>5</v>
@@ -2716,7 +2722,7 @@
         <v>140</v>
       </c>
       <c r="C19" s="43" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>6</v>
@@ -2803,7 +2809,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2849,10 +2855,10 @@
         <v>122</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>167</v>
@@ -2867,7 +2873,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="50" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="28.8">
@@ -2878,7 +2884,7 @@
         <v>169</v>
       </c>
       <c r="C3" s="40" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>7</v>
@@ -2902,7 +2908,7 @@
         <v>170</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>172</v>
@@ -2926,13 +2932,13 @@
         <v>176</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>186</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F5" s="90">
         <v>32</v>
@@ -2950,7 +2956,7 @@
         <v>177</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>188</v>
@@ -2974,7 +2980,7 @@
         <v>178</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>8</v>
@@ -2998,7 +3004,7 @@
         <v>179</v>
       </c>
       <c r="C8" s="40" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>189</v>
@@ -3022,7 +3028,7 @@
         <v>180</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>9</v>
@@ -3048,7 +3054,7 @@
         <v>190</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>10</v>
@@ -3072,7 +3078,7 @@
         <v>191</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>11</v>
@@ -3093,10 +3099,10 @@
     <row r="12" spans="1:8" s="5" customFormat="1">
       <c r="A12" s="36"/>
       <c r="B12" s="36" t="s">
-        <v>190</v>
+        <v>305</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>12</v>
@@ -3122,7 +3128,7 @@
         <v>193</v>
       </c>
       <c r="C13" s="40" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>13</v>
@@ -3146,7 +3152,7 @@
         <v>196</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D14" s="20" t="s">
         <v>197</v>
@@ -3172,7 +3178,7 @@
         <v>206</v>
       </c>
       <c r="C15" s="56" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>198</v>
@@ -3187,7 +3193,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="59" t="s">
-        <v>215</v>
+        <v>304</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="11" customFormat="1">
@@ -3198,7 +3204,7 @@
         <v>207</v>
       </c>
       <c r="C16" s="56" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>199</v>
@@ -3212,8 +3218,8 @@
       <c r="G16" s="60">
         <v>1</v>
       </c>
-      <c r="H16" s="59" t="s">
-        <v>215</v>
+      <c r="H16" s="11" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="14" customFormat="1">
@@ -3224,7 +3230,7 @@
         <v>208</v>
       </c>
       <c r="C17" s="40" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D17" s="67" t="s">
         <v>200</v>
@@ -3237,7 +3243,7 @@
         <v>147</v>
       </c>
       <c r="H17" s="51" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -3246,20 +3252,20 @@
         <v>209</v>
       </c>
       <c r="C18" s="40" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D18" s="67" t="s">
         <v>201</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F18" s="41"/>
       <c r="G18" s="24" t="s">
         <v>147</v>
       </c>
       <c r="H18" s="51" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="22" customFormat="1" ht="15" thickBot="1">
@@ -3268,7 +3274,7 @@
         <v>210</v>
       </c>
       <c r="C19" s="43" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D19" s="68" t="s">
         <v>202</v>
@@ -3283,14 +3289,14 @@
         <v>147</v>
       </c>
       <c r="H19" s="46" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="G20" s="8"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F6" xr:uid="{CC38DCCA-91FB-4098-BDF4-6975A85A75DB}">
       <formula1>"Ja,Nee"</formula1>
     </dataValidation>
@@ -3298,7 +3304,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="8">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2AEE1401-8967-43A0-BCB6-2A69A187890F}">
           <x14:formula1>
             <xm:f>Waardelijsten!$H$2:$H$4</xm:f>
@@ -3401,16 +3407,16 @@
     </row>
     <row r="2" spans="1:8" ht="28.8">
       <c r="A2" s="29" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="B2" s="29" t="s">
-        <v>222</v>
-      </c>
       <c r="C2" s="29" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>168</v>
@@ -3420,19 +3426,19 @@
         <v>1</v>
       </c>
       <c r="H2" s="32" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="5" customFormat="1" ht="28.8">
       <c r="A3" s="36"/>
       <c r="B3" s="36" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C3" s="36" t="s">
         <v>146</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>126</v>
@@ -3444,21 +3450,21 @@
         <v>1</v>
       </c>
       <c r="H3" s="39" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.8">
       <c r="A4" s="29" t="s">
+        <v>229</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>281</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>230</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>226</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>282</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>231</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>168</v>
@@ -3468,16 +3474,16 @@
         <v>1</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.8">
       <c r="A5" s="29"/>
       <c r="B5" s="29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>14</v>
@@ -3490,16 +3496,16 @@
         <v>1</v>
       </c>
       <c r="H5" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.8">
       <c r="A6" s="29"/>
       <c r="B6" s="29" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>15</v>
@@ -3512,19 +3518,19 @@
         <v>1</v>
       </c>
       <c r="H6" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="22" customFormat="1" ht="15" thickBot="1">
       <c r="A7" s="43"/>
       <c r="B7" s="43" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C7" s="43" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E7" s="21" t="s">
         <v>187</v>
@@ -3534,7 +3540,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="46" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -3614,13 +3620,13 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="40" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B2" s="40" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>16</v>
@@ -3633,29 +3639,29 @@
         <v>1</v>
       </c>
       <c r="H2" s="51" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="22" customFormat="1" ht="29.4" thickBot="1">
       <c r="A3" s="43"/>
       <c r="B3" s="43" t="s">
+        <v>239</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>282</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="C3" s="43" t="s">
-        <v>283</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="21" t="s">
         <v>241</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>242</v>
       </c>
       <c r="F3" s="65"/>
       <c r="G3" s="25">
         <v>1</v>
       </c>
       <c r="H3" s="46" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -3683,7 +3689,9 @@
   </sheetPr>
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -3761,7 +3769,7 @@
     </row>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
@@ -3809,12 +3817,12 @@
         <v>24</v>
       </c>
       <c r="Q2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B3" t="s">
         <v>29</v>
@@ -3867,7 +3875,7 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B4" t="s">
         <v>43</v>
@@ -3911,7 +3919,7 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B5" t="s">
         <v>55</v>
@@ -3923,13 +3931,13 @@
         <v>57</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="G5" t="s">
         <v>59</v>
       </c>
       <c r="H5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J5" t="s">
         <v>58</v>
@@ -3946,7 +3954,7 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B6" t="s">
         <v>62</v>
@@ -3958,7 +3966,7 @@
         <v>64</v>
       </c>
       <c r="E6" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="G6" t="s">
         <v>66</v>
@@ -3978,13 +3986,13 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B7" t="s">
         <v>70</v>
       </c>
       <c r="E7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G7" t="s">
         <v>72</v>
@@ -4004,7 +4012,7 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B8" t="s">
         <v>76</v>
@@ -4027,7 +4035,7 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B9" t="s">
         <v>82</v>
@@ -4050,7 +4058,7 @@
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
@@ -4124,7 +4132,7 @@
         <v>99</v>
       </c>
       <c r="Q14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="15" spans="1:17">

</xml_diff>